<commit_message>
Update of PS1 calculation modeled values
</commit_message>
<xml_diff>
--- a/figure07_maps_10Be_model_data_antarctica/model_data_comp_mean_10Be_flux_data_holocene_final.xlsx
+++ b/figure07_maps_10Be_model_data_antarctica/model_data_comp_mean_10Be_flux_data_holocene_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acauquoin/Documents/Mes_manuscrits/10Be_Holocene_Antarctica/figures/figure06_maps_10Be_model_data_antarctica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acauquoin/Documents/Mes_manuscrits/10Be_Holocene_Antarctica/figures/figure07_maps_10Be_model_data_antarctica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224CC8CF-940E-D144-AA82-0C7564EC47AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC855272-207E-424D-8215-2CA5B3476B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="3660" windowWidth="31560" windowHeight="16440" xr2:uid="{E2820EBF-6D30-244A-9364-248DB28BA56B}"/>
+    <workbookView xWindow="64160" yWindow="7520" windowWidth="31560" windowHeight="16440" xr2:uid="{E2820EBF-6D30-244A-9364-248DB28BA56B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,29 +763,29 @@
         <v>107.83866057838662</v>
       </c>
       <c r="E4" s="15">
-        <v>0.39900000000000002</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="F4" s="1">
-        <v>5.28</v>
+        <v>5.77</v>
       </c>
       <c r="G4" s="1">
-        <v>66.88</v>
+        <v>78.7</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" si="2"/>
-        <v>31.746031746031743</v>
+        <v>32.017640214481581</v>
       </c>
       <c r="I4" s="18">
         <f t="shared" si="3"/>
-        <v>1.023076923076923</v>
+        <v>1.0923076923076922</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" si="4"/>
-        <v>0.60550458715596334</v>
+        <v>0.66169724770642191</v>
       </c>
       <c r="K4" s="21">
         <f t="shared" si="5"/>
-        <v>0.62018574453069852</v>
+        <v>0.72979393083980226</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1152,7 +1152,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="13">
         <f>AVERAGE(G2:G12)</f>
-        <v>73.216363636363639</v>
+        <v>74.290909090909082</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="8"/>

</xml_diff>